<commit_message>
Working on screen scrolling, partially implemented
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Survival of the Fittest - Bug Tracking</t>
   </si>
@@ -73,6 +72,18 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>Camera moves with primary character, but that includes movement on the y axis, revealing edges of the map</t>
+  </si>
+  <si>
+    <t>Code - Function</t>
+  </si>
+  <si>
+    <t>Players hitting walls, while holding left or right, refuse to fall via gravity, until the direction is not being held</t>
+  </si>
+  <si>
+    <t>Finder</t>
   </si>
 </sst>
 </file>
@@ -228,7 +239,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,7 +253,37 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
@@ -251,31 +292,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -563,405 +580,614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="1" customWidth="1"/>
-    <col min="6" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="17.7109375" style="1" customWidth="1"/>
-    <col min="14" max="17" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="1" customWidth="1"/>
+    <col min="7" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="15" max="18" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
-      <c r="K4" s="13" t="s">
+      <c r="K4" s="12"/>
+      <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="P4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="Q4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="R4" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5" s="4">
         <v>42468</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="3"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="11"/>
-    </row>
-    <row r="6" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="3"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="8"/>
+    </row>
+    <row r="6" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="10">
         <v>42469</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="E6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="G6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="15">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="10">
         <v>42469</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:17" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="6:10" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
+    <row r="7" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="11">
+        <v>42475</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="11">
+        <v>42475</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="6"/>
+    </row>
+    <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="6"/>
+    </row>
+    <row r="20" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="6"/>
+    </row>
+    <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="6"/>
+    </row>
+    <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="6"/>
+    </row>
+    <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="6"/>
+    </row>
+    <row r="27" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="6"/>
+    </row>
+    <row r="28" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="6"/>
+    </row>
+    <row r="30" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="6"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="F32:J32"/>
-    <mergeCell ref="F33:J33"/>
-    <mergeCell ref="F34:J34"/>
-    <mergeCell ref="F35:J35"/>
-    <mergeCell ref="F36:J36"/>
-    <mergeCell ref="F31:J31"/>
-    <mergeCell ref="F20:J20"/>
-    <mergeCell ref="F21:J21"/>
-    <mergeCell ref="F22:J22"/>
-    <mergeCell ref="F23:J23"/>
-    <mergeCell ref="F24:J24"/>
-    <mergeCell ref="F25:J25"/>
-    <mergeCell ref="F26:J26"/>
-    <mergeCell ref="F27:J27"/>
-    <mergeCell ref="F28:J28"/>
-    <mergeCell ref="F29:J29"/>
-    <mergeCell ref="F30:J30"/>
-    <mergeCell ref="F19:J19"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="F11:J11"/>
-    <mergeCell ref="F12:J12"/>
-    <mergeCell ref="F13:J13"/>
-    <mergeCell ref="F14:J14"/>
-    <mergeCell ref="F15:J15"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="F17:J17"/>
-    <mergeCell ref="F18:J18"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="A1:K3"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="G29:K29"/>
+    <mergeCell ref="G30:K30"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A1:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Player now falls when holding horizontal directions on walls
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -239,7 +239,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,11 +268,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -280,19 +277,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -583,7 +580,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,48 +596,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -661,13 +658,13 @@
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
       <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
@@ -684,7 +681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="80.099999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -703,117 +700,121 @@
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="3"/>
       <c r="O5" s="5"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="8"/>
     </row>
-    <row r="6" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
         <v>2</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="16">
         <v>42469</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="10">
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="16">
         <v>42469</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+    <row r="7" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <v>3</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="16">
         <v>42475</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="16">
+        <v>42478</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
         <v>4</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="16">
         <v>42475</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="16">
+        <v>42480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -823,11 +824,11 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -837,11 +838,11 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -851,11 +852,11 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,11 +866,11 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -879,11 +880,11 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -893,11 +894,11 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -907,11 +908,11 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -921,11 +922,11 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -935,11 +936,11 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -949,11 +950,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -963,11 +964,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -977,11 +978,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -991,11 +992,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1005,11 +1006,11 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1019,11 +1020,11 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1033,11 +1034,11 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1047,11 +1048,11 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1061,11 +1062,11 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1075,11 +1076,11 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1089,11 +1090,11 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1103,62 +1104,74 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G18:K18"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="G21:K21"/>
@@ -1171,23 +1184,11 @@
     <mergeCell ref="G28:K28"/>
     <mergeCell ref="G29:K29"/>
     <mergeCell ref="G30:K30"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="G36:K36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Respawning doesn't work quite yet, near full implementation though
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geeks\OneDrive\College\Penn State\Spring 2016\IST 446\IST446-SotF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\GitHub\IST446-SotF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Survival of the Fittest - Bug Tracking</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Finder</t>
+  </si>
+  <si>
+    <t>Player doesn't repsawn at designated checkpoint after death</t>
   </si>
 </sst>
 </file>
@@ -239,7 +242,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,28 +271,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -579,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:L8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,48 +605,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -658,13 +667,13 @@
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
       <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
@@ -700,13 +709,13 @@
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="3"/>
       <c r="O5" s="5"/>
       <c r="P5" s="3"/>
@@ -714,108 +723,122 @@
       <c r="R5" s="8"/>
     </row>
     <row r="6" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15">
+      <c r="A6" s="10">
         <v>2</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="11">
         <v>42469</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="16">
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="11">
         <v>42469</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
+      <c r="A7" s="10">
         <v>3</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="11">
         <v>42475</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="16">
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="11">
         <v>42478</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15">
+      <c r="A8" s="10">
         <v>4</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="11">
         <v>42475</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="16">
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="11">
         <v>42480</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="6"/>
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="18">
+        <v>42480</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
@@ -824,11 +847,11 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -838,11 +861,11 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -852,11 +875,11 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -866,11 +889,11 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -880,11 +903,11 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -894,11 +917,11 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -908,11 +931,11 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -922,11 +945,11 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -936,11 +959,11 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -950,11 +973,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -964,11 +987,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -978,11 +1001,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -992,11 +1015,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1006,11 +1029,11 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1020,11 +1043,11 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1034,11 +1057,11 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1048,11 +1071,11 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1062,11 +1085,11 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1076,11 +1099,11 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1090,11 +1113,11 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1104,62 +1127,74 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="G29:K29"/>
+    <mergeCell ref="G30:K30"/>
     <mergeCell ref="G19:K19"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="G9:K9"/>
@@ -1172,23 +1207,11 @@
     <mergeCell ref="G16:K16"/>
     <mergeCell ref="G17:K17"/>
     <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="G29:K29"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A1:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Full controller support, multiple players now working in all cases. NOTE - Test for 3 and 4 players yet
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>Survival of the Fittest - Bug Tracking</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Game fails to recognize the first player past the finish line</t>
+  </si>
+  <si>
+    <t>Switching to gamepad controls allows the player to jump infinitely</t>
+  </si>
+  <si>
+    <t>Players 1 and 2 move in unison</t>
   </si>
 </sst>
 </file>
@@ -280,23 +286,23 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -585,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,48 +608,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -664,13 +670,13 @@
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
@@ -706,13 +712,13 @@
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="3"/>
       <c r="O5" s="5"/>
       <c r="P5" s="3"/>
@@ -869,46 +875,78 @@
         <v>42481</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="6"/>
-    </row>
-    <row r="12" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="6"/>
-    </row>
-    <row r="13" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>7</v>
+      </c>
+      <c r="B11" s="11">
+        <v>42482</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="11">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>8</v>
+      </c>
+      <c r="B12" s="11">
+        <v>42482</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="11">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -918,11 +956,11 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -932,11 +970,11 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -946,11 +984,11 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -960,11 +998,11 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -974,11 +1012,11 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -988,11 +1026,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1002,11 +1040,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1016,11 +1054,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1030,11 +1068,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1044,11 +1082,11 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1058,11 +1096,11 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1072,11 +1110,11 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1086,11 +1124,11 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1100,11 +1138,11 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1114,11 +1152,11 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1128,11 +1166,11 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1142,62 +1180,74 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G18:K18"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="G21:K21"/>
@@ -1210,23 +1260,11 @@
     <mergeCell ref="G28:K28"/>
     <mergeCell ref="G29:K29"/>
     <mergeCell ref="G30:K30"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="G36:K36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
4 Players now confirmed working; full controlls working, respawning works for all characters
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
   <si>
     <t>Survival of the Fittest - Bug Tracking</t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>Player 2 on respawn doesn't die from gun fire</t>
+  </si>
+  <si>
+    <t>Only players 1 and 2 respawn after death, even with 4 players</t>
+  </si>
+  <si>
+    <t>On respawn, player 4 respawns twice if all 4 players die</t>
+  </si>
+  <si>
+    <t>Player 3 respawned when still alive at respawn</t>
+  </si>
+  <si>
+    <t>If Player 1 is the only one alive, the game fully crashes</t>
   </si>
 </sst>
 </file>
@@ -254,7 +266,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -289,29 +301,23 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -600,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,48 +623,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -679,13 +685,13 @@
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
       <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
@@ -721,13 +727,13 @@
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
       <c r="L5" s="3"/>
       <c r="O5" s="5"/>
       <c r="P5" s="3"/>
@@ -944,102 +950,168 @@
         <v>42482</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>9</v>
-      </c>
-      <c r="B13" s="18">
+    <row r="13" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11">
         <v>42482</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="19" t="s">
+      <c r="F13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="6"/>
-    </row>
-    <row r="15" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="6"/>
-    </row>
-    <row r="16" spans="1:18" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="11">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11">
+        <v>42482</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="11">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>11</v>
+      </c>
+      <c r="B15" s="11">
+        <v>42482</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="11">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>12</v>
+      </c>
+      <c r="B16" s="11">
+        <v>42482</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="11">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <v>13</v>
+      </c>
+      <c r="B17" s="11">
+        <v>42482</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="11">
+        <v>42482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1049,11 +1121,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,11 +1135,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1077,11 +1149,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1091,11 +1163,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1105,11 +1177,11 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1119,11 +1191,11 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1133,11 +1205,11 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1147,11 +1219,11 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1161,11 +1233,11 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1175,11 +1247,11 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1189,11 +1261,11 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1203,62 +1275,74 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G18:K18"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="G21:K21"/>
@@ -1271,23 +1355,11 @@
     <mergeCell ref="G28:K28"/>
     <mergeCell ref="G29:K29"/>
     <mergeCell ref="G30:K30"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="G36:K36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Started on title screen, 1 of 3 buttons shows, for some reason
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geeks\Downloads\IST446-SotF-master\IST446-SotF-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f8ef1c534562f43/College/Penn State/Spring 2016/IST 446/IST446-SotF/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
   <si>
     <t>Survival of the Fittest - Bug Tracking</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>If Player 1 is the only one alive, the game fully crashes</t>
+  </si>
+  <si>
+    <t>Menu only displays 1 button instad of 3</t>
   </si>
 </sst>
 </file>
@@ -266,7 +269,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -301,23 +304,29 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -607,7 +616,7 @@
   <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,48 +632,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -685,13 +694,13 @@
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
       <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
@@ -727,13 +736,13 @@
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
       <c r="L5" s="3"/>
       <c r="O5" s="5"/>
       <c r="P5" s="3"/>
@@ -1101,18 +1110,32 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="6"/>
+      <c r="A18" s="7">
+        <v>14</v>
+      </c>
+      <c r="B18" s="18">
+        <v>42484</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="7"/>
     </row>
     <row r="19" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
@@ -1121,11 +1144,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1135,11 +1158,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1149,11 +1172,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1163,11 +1186,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1177,11 +1200,11 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1191,11 +1214,11 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1205,11 +1228,11 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1219,11 +1242,11 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1233,11 +1256,11 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1247,11 +1270,11 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1261,11 +1284,11 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1275,62 +1298,74 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G31:K31"/>
+    <mergeCell ref="G20:K20"/>
+    <mergeCell ref="G21:K21"/>
+    <mergeCell ref="G22:K22"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G26:K26"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G28:K28"/>
+    <mergeCell ref="G29:K29"/>
+    <mergeCell ref="G30:K30"/>
     <mergeCell ref="G19:K19"/>
     <mergeCell ref="G8:K8"/>
     <mergeCell ref="G9:K9"/>
@@ -1343,23 +1378,11 @@
     <mergeCell ref="G16:K16"/>
     <mergeCell ref="G17:K17"/>
     <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G31:K31"/>
-    <mergeCell ref="G20:K20"/>
-    <mergeCell ref="G21:K21"/>
-    <mergeCell ref="G22:K22"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="G26:K26"/>
-    <mergeCell ref="G27:K27"/>
-    <mergeCell ref="G28:K28"/>
-    <mergeCell ref="G29:K29"/>
-    <mergeCell ref="G30:K30"/>
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A1:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Main menu works, no controller support for menu, try to fix maybe
</commit_message>
<xml_diff>
--- a/Bugs.xlsx
+++ b/Bugs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f8ef1c534562f43/College/Penn State/Spring 2016/IST 446/IST446-SotF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Documents\GitHub\IST446-SotF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="31">
   <si>
     <t>Survival of the Fittest - Bug Tracking</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Menu only displays 1 button instad of 3</t>
+  </si>
+  <si>
+    <t>Clicking play from the menu starts the game, but the level acts as if it started playing when the menu started</t>
   </si>
 </sst>
 </file>
@@ -304,29 +307,29 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -615,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,48 +635,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
@@ -694,13 +697,13 @@
       <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="9" t="s">
         <v>12</v>
       </c>
@@ -736,13 +739,13 @@
       <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
       <c r="L5" s="3"/>
       <c r="O5" s="5"/>
       <c r="P5" s="3"/>
@@ -768,13 +771,13 @@
       <c r="F6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
       <c r="L6" s="11">
         <v>42469</v>
       </c>
@@ -798,13 +801,13 @@
       <c r="F7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="11">
         <v>42478</v>
       </c>
@@ -828,13 +831,13 @@
       <c r="F8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="11">
         <v>42480</v>
       </c>
@@ -858,13 +861,13 @@
       <c r="F9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
       <c r="L9" s="11">
         <v>42481</v>
       </c>
@@ -888,13 +891,13 @@
       <c r="F10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
       <c r="L10" s="11">
         <v>42481</v>
       </c>
@@ -918,13 +921,13 @@
       <c r="F11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="11">
         <v>42482</v>
       </c>
@@ -948,13 +951,13 @@
       <c r="F12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="11">
         <v>42482</v>
       </c>
@@ -978,13 +981,13 @@
       <c r="F13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
       <c r="L13" s="11">
         <v>42482</v>
       </c>
@@ -1008,13 +1011,13 @@
       <c r="F14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
       <c r="L14" s="11">
         <v>42482</v>
       </c>
@@ -1038,13 +1041,13 @@
       <c r="F15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
       <c r="L15" s="11">
         <v>42482</v>
       </c>
@@ -1068,13 +1071,13 @@
       <c r="F16" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
       <c r="L16" s="11">
         <v>42482</v>
       </c>
@@ -1098,58 +1101,74 @@
       <c r="F17" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="11">
         <v>42482</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+    <row r="18" spans="1:12" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
         <v>14</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="11">
         <v>42484</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="19" t="s">
+      <c r="F18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="6"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="11">
+        <v>42484</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>15</v>
+      </c>
+      <c r="B19" s="12">
+        <v>42484</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
@@ -1158,11 +1177,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1172,11 +1191,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1186,11 +1205,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1200,11 +1219,11 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1214,11 +1233,11 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1228,11 +1247,11 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1242,11 +1261,11 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1256,11 +1275,11 @@
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1270,11 +1289,11 @@
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1284,11 +1303,11 @@
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="1:12" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -1298,62 +1317,74 @@
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="17"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G32:K32"/>
-    <mergeCell ref="G33:K33"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="G36:K36"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="G5:K5"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G19:K19"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="G15:K15"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G18:K18"/>
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="G20:K20"/>
     <mergeCell ref="G21:K21"/>
@@ -1366,23 +1397,11 @@
     <mergeCell ref="G28:K28"/>
     <mergeCell ref="G29:K29"/>
     <mergeCell ref="G30:K30"/>
-    <mergeCell ref="G19:K19"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="G13:K13"/>
-    <mergeCell ref="G14:K14"/>
-    <mergeCell ref="G15:K15"/>
-    <mergeCell ref="G16:K16"/>
-    <mergeCell ref="G17:K17"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="G5:K5"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="A1:L3"/>
+    <mergeCell ref="G32:K32"/>
+    <mergeCell ref="G33:K33"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="G36:K36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>